<commit_message>
feat(client) add LD46 creature screenshot to rules
</commit_message>
<xml_diff>
--- a/packages/ld46/docs/cards/Creatures.xlsx
+++ b/packages/ld46/docs/cards/Creatures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\jou\packages\ld46\docs\cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2C9418-FB36-4FCC-9A57-D4DA74D4B618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4923AF0-0DAC-43A7-B2AD-42D24B51A828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10110" yWindow="4065" windowWidth="19155" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7680" yWindow="1215" windowWidth="19155" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>bg</t>
   </si>
@@ -110,12 +110,6 @@
     <t>special</t>
   </si>
   <si>
-    <t>No special</t>
-  </si>
-  <si>
-    <t>+3 Excitement each turn the chariot remains in play</t>
-  </si>
-  <si>
     <t>Lion</t>
   </si>
   <si>
@@ -134,24 +128,6 @@
     <t>Wolf Pack</t>
   </si>
   <si>
-    <t>One additional 3 CP "stomp" attack per turn</t>
-  </si>
-  <si>
-    <t>At the start of each turn, randomly SLOW one player for that turn.</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>lion.png</t>
   </si>
   <si>
@@ -171,6 +147,72 @@
   </si>
   <si>
     <t>chariot.png</t>
+  </si>
+  <si>
+    <t>2 / 3</t>
+  </si>
+  <si>
+    <t>3 / 4</t>
+  </si>
+  <si>
+    <t>3 / 5</t>
+  </si>
+  <si>
+    <t>4 / 6</t>
+  </si>
+  <si>
+    <t>2 / 4</t>
+  </si>
+  <si>
+    <t>5 / 7</t>
+  </si>
+  <si>
+    <t>4 / 7</t>
+  </si>
+  <si>
+    <t>3 / 6</t>
+  </si>
+  <si>
+    <t>5 / 8</t>
+  </si>
+  <si>
+    <t>5 / 6</t>
+  </si>
+  <si>
+    <t>6 / 7</t>
+  </si>
+  <si>
+    <t>7 / 8</t>
+  </si>
+  <si>
+    <t>6 / 8</t>
+  </si>
+  <si>
+    <t>7 / 9</t>
+  </si>
+  <si>
+    <t>4 / 5</t>
+  </si>
+  <si>
+    <t>LARGE</t>
+  </si>
+  <si>
+    <t>LARGE, ARMOURED, One additional 3 CP "stomp" attack per turn</t>
+  </si>
+  <si>
+    <t>PACK. At the start of each turn, randomly SLOW one player for that turn. +1 CP vs SLOW.</t>
+  </si>
+  <si>
+    <t>PACK.</t>
+  </si>
+  <si>
+    <t>Cannot be SLOWED. +3 Excitement each turn the chariot remains in play</t>
+  </si>
+  <si>
+    <t>ARMOURED</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -206,180 +248,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -661,7 +552,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,9 +562,9 @@
     <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="6" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -701,10 +592,10 @@
       <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -725,7 +616,7 @@
       <c r="P1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -760,26 +651,26 @@
       <c r="J2">
         <v>8</v>
       </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
-      <c r="L2">
-        <v>3</v>
-      </c>
-      <c r="M2">
-        <v>4</v>
-      </c>
-      <c r="N2">
-        <v>4</v>
-      </c>
-      <c r="O2">
-        <v>5</v>
-      </c>
-      <c r="P2">
-        <v>6</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>24</v>
+      <c r="K2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -819,32 +710,26 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="N3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="O3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="P3">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>24</v>
+      <c r="K3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -852,7 +737,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -884,32 +769,26 @@
         <f t="shared" ref="J4" si="5">+J3+1</f>
         <v>10</v>
       </c>
-      <c r="K4">
-        <f t="shared" ref="K4" si="6">+K3+1</f>
-        <v>5</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ref="L4" si="7">+L3+1</f>
-        <v>5</v>
-      </c>
-      <c r="M4">
-        <f t="shared" ref="M4" si="8">+M3+1</f>
-        <v>6</v>
-      </c>
-      <c r="N4">
-        <f t="shared" ref="N4" si="9">+N3+1</f>
-        <v>6</v>
-      </c>
-      <c r="O4">
-        <f t="shared" ref="O4" si="10">+O3+1</f>
-        <v>7</v>
-      </c>
-      <c r="P4">
-        <f t="shared" ref="P4" si="11">+P3+1</f>
-        <v>8</v>
-      </c>
-      <c r="Q4" s="2" t="s">
+      <c r="K4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>40</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -930,51 +809,45 @@
         <v>7</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5" si="12">+F3+1</f>
+        <f t="shared" ref="F5" si="6">+F3+1</f>
         <v>8</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5" si="13">+G3+1</f>
+        <f t="shared" ref="G5" si="7">+G3+1</f>
         <v>8</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5" si="14">+H3+1</f>
+        <f t="shared" ref="H5" si="8">+H3+1</f>
         <v>9</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5" si="15">+I3+1</f>
+        <f t="shared" ref="I5" si="9">+I3+1</f>
         <v>9</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5" si="16">+J3+1</f>
+        <f t="shared" ref="J5" si="10">+J3+1</f>
         <v>10</v>
       </c>
-      <c r="K5">
-        <f t="shared" ref="K5" si="17">+K3+1</f>
-        <v>5</v>
-      </c>
-      <c r="L5">
-        <f t="shared" ref="L5" si="18">+L3+1</f>
-        <v>5</v>
-      </c>
-      <c r="M5">
-        <f t="shared" ref="M5" si="19">+M3+1</f>
-        <v>6</v>
-      </c>
-      <c r="N5">
-        <f t="shared" ref="N5" si="20">+N3+1</f>
-        <v>6</v>
-      </c>
-      <c r="O5">
-        <f t="shared" ref="O5" si="21">+O3+1</f>
-        <v>7</v>
-      </c>
-      <c r="P5">
-        <f t="shared" ref="P5" si="22">+P3+1</f>
-        <v>8</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>24</v>
+      <c r="K5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -988,7 +861,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>8</v>
@@ -1002,32 +875,32 @@
       <c r="H6">
         <v>10</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>11</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>12</v>
       </c>
-      <c r="K6" s="3">
-        <v>6</v>
-      </c>
-      <c r="L6" s="3">
-        <v>7</v>
-      </c>
-      <c r="M6" s="3">
-        <v>7</v>
-      </c>
-      <c r="N6" s="3">
-        <v>8</v>
-      </c>
-      <c r="O6" s="3">
-        <v>8</v>
-      </c>
-      <c r="P6" s="3">
-        <v>9</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>25</v>
+      <c r="K6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1035,78 +908,78 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <f>E3</f>
         <v>6</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:P7" si="23">F3</f>
+        <f t="shared" ref="F7:P7" si="11">F3</f>
         <v>7</v>
       </c>
       <c r="G7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="H7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="I7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="J7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="23"/>
-        <v>4</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="23"/>
-        <v>4</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="23"/>
-        <v>5</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="23"/>
-        <v>5</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="23"/>
-        <v>6</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="23"/>
-        <v>7</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>30</v>
+      <c r="K7" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>2 / 4</v>
+      </c>
+      <c r="L7" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>3 / 4</v>
+      </c>
+      <c r="M7" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>3 / 5</v>
+      </c>
+      <c r="N7" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>3 / 5</v>
+      </c>
+      <c r="O7" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>4 / 6</v>
+      </c>
+      <c r="P7" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>4 / 7</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -1126,105 +999,99 @@
       <c r="J8">
         <v>8</v>
       </c>
-      <c r="K8">
-        <v>3</v>
-      </c>
-      <c r="L8">
-        <v>3</v>
-      </c>
-      <c r="M8">
-        <v>4</v>
-      </c>
-      <c r="N8">
-        <v>4</v>
-      </c>
-      <c r="O8">
-        <v>5</v>
-      </c>
-      <c r="P8">
-        <v>6</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>33</v>
+      <c r="K8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E9">
         <f>+E8+1</f>
         <v>6</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9" si="24">+F8+1</f>
+        <f t="shared" ref="F9" si="12">+F8+1</f>
         <v>7</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G9" si="25">+G8+1</f>
+        <f t="shared" ref="G9" si="13">+G8+1</f>
         <v>7</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9" si="26">+H8+1</f>
+        <f t="shared" ref="H9" si="14">+H8+1</f>
         <v>8</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I9" si="27">+I8+1</f>
+        <f t="shared" ref="I9" si="15">+I8+1</f>
         <v>8</v>
       </c>
       <c r="J9">
-        <f t="shared" ref="J9" si="28">+J8+1</f>
+        <f t="shared" ref="J9" si="16">+J8+1</f>
         <v>9</v>
       </c>
-      <c r="K9">
-        <f t="shared" ref="K9" si="29">+K8+1</f>
-        <v>4</v>
-      </c>
-      <c r="L9">
-        <f t="shared" ref="L9" si="30">+L8+1</f>
-        <v>4</v>
-      </c>
-      <c r="M9">
-        <f t="shared" ref="M9" si="31">+M8+1</f>
-        <v>5</v>
-      </c>
-      <c r="N9">
-        <f t="shared" ref="N9" si="32">+N8+1</f>
-        <v>5</v>
-      </c>
-      <c r="O9">
-        <f t="shared" ref="O9" si="33">+O8+1</f>
-        <v>6</v>
-      </c>
-      <c r="P9">
-        <f t="shared" ref="P9" si="34">+P8+1</f>
-        <v>7</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>24</v>
+      <c r="K9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -1238,38 +1105,38 @@
       <c r="H10">
         <v>8</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>9</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>9</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="3" t="str">
         <f>K5</f>
-        <v>5</v>
-      </c>
-      <c r="L10">
-        <f t="shared" ref="L10:P10" si="35">L5</f>
-        <v>5</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="35"/>
-        <v>6</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="35"/>
-        <v>6</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="35"/>
-        <v>7</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="35"/>
-        <v>8</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>32</v>
+        <v>3 / 5</v>
+      </c>
+      <c r="L10" s="3" t="str">
+        <f t="shared" ref="L10:P10" si="17">L5</f>
+        <v>3 / 6</v>
+      </c>
+      <c r="M10" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>4 / 6</v>
+      </c>
+      <c r="N10" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>4 / 6</v>
+      </c>
+      <c r="O10" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>5 / 7</v>
+      </c>
+      <c r="P10" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>5 / 8</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(client) numerous bug fixes, "game" works
</commit_message>
<xml_diff>
--- a/packages/ld46/docs/cards/Creatures.xlsx
+++ b/packages/ld46/docs/cards/Creatures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\jou\packages\ld46\docs\cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4923AF0-0DAC-43A7-B2AD-42D24B51A828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B7891C-21C3-4872-BA3A-8C7312C1347E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7680" yWindow="1215" windowWidth="19155" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>bg</t>
   </si>
@@ -147,51 +147,6 @@
   </si>
   <si>
     <t>chariot.png</t>
-  </si>
-  <si>
-    <t>2 / 3</t>
-  </si>
-  <si>
-    <t>3 / 4</t>
-  </si>
-  <si>
-    <t>3 / 5</t>
-  </si>
-  <si>
-    <t>4 / 6</t>
-  </si>
-  <si>
-    <t>2 / 4</t>
-  </si>
-  <si>
-    <t>5 / 7</t>
-  </si>
-  <si>
-    <t>4 / 7</t>
-  </si>
-  <si>
-    <t>3 / 6</t>
-  </si>
-  <si>
-    <t>5 / 8</t>
-  </si>
-  <si>
-    <t>5 / 6</t>
-  </si>
-  <si>
-    <t>6 / 7</t>
-  </si>
-  <si>
-    <t>7 / 8</t>
-  </si>
-  <si>
-    <t>6 / 8</t>
-  </si>
-  <si>
-    <t>7 / 9</t>
-  </si>
-  <si>
-    <t>4 / 5</t>
   </si>
   <si>
     <t>LARGE</t>
@@ -248,11 +203,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -552,7 +504,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q4" sqref="Q4"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,9 +514,9 @@
     <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="6" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="6" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -592,31 +544,31 @@
       <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -634,43 +586,53 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2">
+        <f t="shared" ref="F2:J2" si="0">$E2+E2</f>
         <v>6</v>
       </c>
       <c r="G2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <f>$K2+K2</f>
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:P2" si="1">$K2+L2</f>
         <v>6</v>
       </c>
-      <c r="H2" s="1">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2">
+      <c r="N2">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="O2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="P2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -688,48 +650,53 @@
       </c>
       <c r="E3">
         <f>+E2+1</f>
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <f>$E3+E3</f>
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <f>$E3+F3</f>
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <f>$E3+G3</f>
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <f>$E3+H3</f>
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <f>$E3+I3</f>
+        <v>24</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:O10" si="2">$K3+K3</f>
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:P3" si="3">$K3+L3</f>
         <v>6</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:P3" si="0">+F2+1</f>
-        <v>7</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H3">
-        <f t="shared" si="0"/>
+      <c r="N3">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" s="4" t="s">
+      <c r="O3">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -747,47 +714,52 @@
       </c>
       <c r="E4">
         <f>+E3+1</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4" si="1">+F3+1</f>
-        <v>8</v>
+        <f t="shared" ref="F4:J4" si="4">$E4+E4</f>
+        <v>10</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4" si="2">+G3+1</f>
-        <v>8</v>
+        <f t="shared" si="4"/>
+        <v>15</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4" si="3">+H3+1</f>
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:P4" si="5">$K4+L4</f>
         <v>9</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4" si="4">+I3+1</f>
-        <v>9</v>
-      </c>
-      <c r="J4">
-        <f t="shared" ref="J4" si="5">+J3+1</f>
-        <v>10</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q4" s="6" t="s">
+      <c r="N4">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="Q4" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -806,48 +778,53 @@
       </c>
       <c r="E5">
         <f>+E3+1</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5" si="6">+F3+1</f>
+        <f t="shared" ref="F5:J5" si="6">$E5+E5</f>
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="K5" s="3">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="G5">
-        <f t="shared" ref="G5" si="7">+G3+1</f>
-        <v>8</v>
-      </c>
-      <c r="H5">
-        <f t="shared" ref="H5" si="8">+H3+1</f>
-        <v>9</v>
-      </c>
-      <c r="I5">
-        <f t="shared" ref="I5" si="9">+I3+1</f>
-        <v>9</v>
-      </c>
-      <c r="J5">
-        <f t="shared" ref="J5" si="10">+J3+1</f>
-        <v>10</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" s="4" t="s">
+      <c r="M5">
+        <f t="shared" ref="M5:P5" si="7">$K5+L5</f>
+        <v>12</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="7"/>
+        <v>24</v>
+      </c>
+      <c r="Q5" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -867,40 +844,50 @@
         <v>8</v>
       </c>
       <c r="F6">
+        <f t="shared" ref="F6:J6" si="8">$E6+E6</f>
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="8"/>
+        <v>32</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="8"/>
+        <v>48</v>
+      </c>
+      <c r="K6" s="2">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="G6">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>10</v>
-      </c>
-      <c r="I6" s="2">
-        <v>11</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="M6">
+        <f t="shared" ref="M6:P6" si="9">$K6+L6</f>
         <v>12</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>56</v>
+      <c r="N6">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -918,53 +905,52 @@
       </c>
       <c r="E7">
         <f>E3</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:P7" si="11">F3</f>
-        <v>7</v>
+        <f t="shared" ref="F7:J7" si="10">$E7+E7</f>
+        <v>8</v>
       </c>
       <c r="G7">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="K7" s="2">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ref="M7:P7" si="11">$K7+L7</f>
+        <v>15</v>
+      </c>
+      <c r="N7">
         <f t="shared" si="11"/>
-        <v>7</v>
-      </c>
-      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="O7">
         <f t="shared" si="11"/>
-        <v>8</v>
-      </c>
-      <c r="I7">
+        <v>25</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="11"/>
-        <v>8</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="11"/>
-        <v>9</v>
-      </c>
-      <c r="K7" s="3" t="str">
-        <f t="shared" si="11"/>
-        <v>2 / 4</v>
-      </c>
-      <c r="L7" s="3" t="str">
-        <f t="shared" si="11"/>
-        <v>3 / 4</v>
-      </c>
-      <c r="M7" s="3" t="str">
-        <f t="shared" si="11"/>
-        <v>3 / 5</v>
-      </c>
-      <c r="N7" s="3" t="str">
-        <f t="shared" si="11"/>
-        <v>3 / 5</v>
-      </c>
-      <c r="O7" s="3" t="str">
-        <f t="shared" si="11"/>
-        <v>4 / 6</v>
-      </c>
-      <c r="P7" s="3" t="str">
-        <f t="shared" si="11"/>
-        <v>4 / 7</v>
-      </c>
-      <c r="Q7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -985,40 +971,50 @@
         <v>5</v>
       </c>
       <c r="F8">
+        <f t="shared" ref="F8:J8" si="12">$E8+E8</f>
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="12"/>
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="12"/>
+        <v>25</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="K8" s="2">
         <v>6</v>
       </c>
-      <c r="G8">
-        <v>6</v>
-      </c>
-      <c r="H8" s="1">
-        <v>7</v>
-      </c>
-      <c r="I8">
-        <v>7</v>
-      </c>
-      <c r="J8">
-        <v>8</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O8" s="3" t="s">
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ref="M8:P8" si="13">$K8+L8</f>
+        <v>18</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="13"/>
+        <v>24</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="13"/>
+        <v>30</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="13"/>
+        <v>36</v>
+      </c>
+      <c r="Q8" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="P8" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1039,45 +1035,50 @@
         <v>6</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9" si="12">+F8+1</f>
-        <v>7</v>
+        <f t="shared" ref="F9:J9" si="14">$E9+E9</f>
+        <v>12</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G9" si="13">+G8+1</f>
-        <v>7</v>
+        <f t="shared" si="14"/>
+        <v>18</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9" si="14">+H8+1</f>
-        <v>8</v>
+        <f t="shared" si="14"/>
+        <v>24</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I9" si="15">+I8+1</f>
-        <v>8</v>
+        <f t="shared" si="14"/>
+        <v>30</v>
       </c>
       <c r="J9">
-        <f t="shared" ref="J9" si="16">+J8+1</f>
-        <v>9</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>52</v>
+        <f t="shared" si="14"/>
+        <v>36</v>
+      </c>
+      <c r="K9" s="2">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9:P9" si="15">$K9+L9</f>
+        <v>18</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="15"/>
+        <v>24</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="15"/>
+        <v>36</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1097,46 +1098,50 @@
         <v>8</v>
       </c>
       <c r="F10">
-        <v>8</v>
+        <f t="shared" ref="F10:J10" si="16">$E10+E10</f>
+        <v>16</v>
       </c>
       <c r="G10">
-        <v>8</v>
+        <f t="shared" si="16"/>
+        <v>24</v>
       </c>
       <c r="H10">
-        <v>8</v>
-      </c>
-      <c r="I10" s="2">
-        <v>9</v>
-      </c>
-      <c r="J10" s="2">
-        <v>9</v>
-      </c>
-      <c r="K10" s="3" t="str">
-        <f>K5</f>
-        <v>3 / 5</v>
-      </c>
-      <c r="L10" s="3" t="str">
-        <f t="shared" ref="L10:P10" si="17">L5</f>
-        <v>3 / 6</v>
-      </c>
-      <c r="M10" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>32</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="16"/>
+        <v>40</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="16"/>
+        <v>48</v>
+      </c>
+      <c r="K10" s="2">
+        <v>7</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10:P10" si="17">$K10+L10</f>
+        <v>21</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="17"/>
-        <v>4 / 6</v>
-      </c>
-      <c r="N10" s="3" t="str">
+        <v>28</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="17"/>
-        <v>4 / 6</v>
-      </c>
-      <c r="O10" s="3" t="str">
+        <v>35</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="17"/>
-        <v>5 / 7</v>
-      </c>
-      <c r="P10" s="3" t="str">
-        <f t="shared" si="17"/>
-        <v>5 / 8</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>53</v>
+        <v>42</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>